<commit_message>
add java proyect Consultor y modif in mainFunc
</commit_message>
<xml_diff>
--- a/workBookOne/mainFunc.xlsx
+++ b/workBookOne/mainFunc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ccc827abb166892/Escritorio/mi proyecto1/workBookOne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{FA623A97-18B9-49ED-B491-CAF2981DEEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EC01663-30BA-433E-936C-013EAD0CBB01}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{FA623A97-18B9-49ED-B491-CAF2981DEEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8699CDD8-E668-4008-A9EF-50592917CF14}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="405" windowWidth="12495" windowHeight="11385" xr2:uid="{CD3A81E2-2964-4D85-BAA7-E2B1FC9C5745}"/>
+    <workbookView xWindow="12435" yWindow="960" windowWidth="12495" windowHeight="11385" xr2:uid="{CD3A81E2-2964-4D85-BAA7-E2B1FC9C5745}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>